<commit_message>
finished adding utyility equations
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C96260-B566-4BAF-AC78-E8B7C0CB269F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863F301A-AE00-45DD-B257-A7CEF6613CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="163">
   <si>
     <t>components</t>
   </si>
@@ -579,7 +579,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -625,6 +625,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,7 +790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -850,6 +856,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2353,6 +2360,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2851,8 +2862,8 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D2" sqref="D2"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2979,8 +2990,8 @@
       <c r="O2" t="s">
         <v>110</v>
       </c>
-      <c r="P2">
-        <v>0</v>
+      <c r="P2" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3035,8 +3046,8 @@
       <c r="O3" t="s">
         <v>110</v>
       </c>
-      <c r="P3">
-        <v>0</v>
+      <c r="P3" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3091,8 +3102,8 @@
       <c r="O4" t="s">
         <v>110</v>
       </c>
-      <c r="P4">
-        <v>0</v>
+      <c r="P4" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -3147,8 +3158,8 @@
       <c r="O5" t="s">
         <v>110</v>
       </c>
-      <c r="P5">
-        <v>0</v>
+      <c r="P5" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -3203,8 +3214,8 @@
       <c r="O6" t="s">
         <v>110</v>
       </c>
-      <c r="P6">
-        <v>0</v>
+      <c r="P6" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -3259,8 +3270,8 @@
       <c r="O7" t="s">
         <v>110</v>
       </c>
-      <c r="P7">
-        <v>0</v>
+      <c r="P7" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -4051,8 +4062,8 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M1" sqref="M1:O1"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4662,7 +4673,7 @@
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="37">
         <v>0</v>
       </c>
       <c r="L11" s="1">
@@ -5081,7 +5092,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B16:J17 B5:D15 K2:R17 B18:R18 E2:J15">
+  <conditionalFormatting sqref="B16:J17 B5:D15 K2:R10 B18:R18 E2:J15 K12:R17 L11:R11">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
added cost of waste (code broken), errors in interval_class
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863F301A-AE00-45DD-B257-A7CEF6613CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9AFD9F-954A-4C55-9EBB-46CFC107218C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="162">
   <si>
     <t>components</t>
   </si>
@@ -359,9 +359,6 @@
   </si>
   <si>
     <t>{'Hoc' : 'liq_liq_ext' }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None </t>
   </si>
   <si>
     <t>[0.01,  0.01, 0.5, 1]</t>
@@ -1078,15 +1075,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
+      <xdr:colOff>34290</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>96520</xdr:rowOff>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>1229360</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>180340</xdr:rowOff>
+      <xdr:colOff>1172210</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2540</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1101,8 +1098,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14386560" y="279400"/>
-          <a:ext cx="1137920" cy="1363980"/>
+          <a:off x="21414740" y="287020"/>
+          <a:ext cx="1137920" cy="1372870"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2767,7 +2764,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2782,7 +2779,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2861,9 +2858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P6" sqref="P6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2893,16 +2890,16 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="D1" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>128</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>129</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>82</v>
@@ -2929,7 +2926,7 @@
         <v>99</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>74</v>
@@ -2952,25 +2949,25 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J2">
         <v>15</v>
@@ -2979,19 +2976,19 @@
         <v>95</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N2">
         <v>0.5</v>
       </c>
       <c r="O2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3008,25 +3005,25 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G3">
         <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J3">
         <v>15</v>
@@ -3035,19 +3032,19 @@
         <v>95</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N3">
         <v>0.5</v>
       </c>
       <c r="O3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3064,25 +3061,25 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G4">
         <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J4">
         <v>15</v>
@@ -3091,19 +3088,19 @@
         <v>95</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N4">
         <v>0.5</v>
       </c>
       <c r="O4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -3120,25 +3117,25 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G5">
         <v>100</v>
       </c>
       <c r="H5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J5">
         <v>15</v>
@@ -3147,19 +3144,19 @@
         <v>95</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N5">
         <v>0.5</v>
       </c>
       <c r="O5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -3176,25 +3173,25 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G6">
         <v>100</v>
       </c>
       <c r="H6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J6">
         <v>15</v>
@@ -3203,19 +3200,19 @@
         <v>95</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N6">
         <v>0.5</v>
       </c>
       <c r="O6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -3232,25 +3229,25 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>132</v>
-      </c>
       <c r="F7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G7">
         <v>100</v>
       </c>
       <c r="H7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J7">
         <v>15</v>
@@ -3262,16 +3259,16 @@
         <v>54</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N7">
         <v>0.5</v>
       </c>
       <c r="O7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -3288,10 +3285,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E8" s="33">
         <v>0</v>
@@ -3303,19 +3300,19 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>98</v>
       </c>
       <c r="J8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K8" t="s">
         <v>95</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>106</v>
+      <c r="L8" s="5">
+        <v>0</v>
       </c>
       <c r="M8" s="5">
         <v>0</v>
@@ -3324,10 +3321,10 @@
         <v>0.5</v>
       </c>
       <c r="O8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -3344,7 +3341,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>97</v>
@@ -3371,8 +3368,8 @@
       <c r="K9" t="s">
         <v>95</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>106</v>
+      <c r="L9" s="5">
+        <v>0</v>
       </c>
       <c r="M9" s="5">
         <v>0</v>
@@ -3381,10 +3378,10 @@
         <v>0.5</v>
       </c>
       <c r="O9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -3395,16 +3392,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="33">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E10" s="33">
         <v>0</v>
@@ -3427,8 +3424,8 @@
       <c r="K10" t="s">
         <v>95</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>106</v>
+      <c r="L10" s="5">
+        <v>0</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>101</v>
@@ -3437,10 +3434,10 @@
         <v>0.5</v>
       </c>
       <c r="O10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -3451,16 +3448,16 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" s="33">
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E11" s="33">
         <v>0</v>
@@ -3483,8 +3480,8 @@
       <c r="K11" t="s">
         <v>95</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>106</v>
+      <c r="L11" s="5">
+        <v>0</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>100</v>
@@ -3493,10 +3490,10 @@
         <v>0.5</v>
       </c>
       <c r="O11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -3507,16 +3504,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B12" s="33">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E12" s="33">
         <v>0</v>
@@ -3539,8 +3536,8 @@
       <c r="K12" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>106</v>
+      <c r="L12" s="5">
+        <v>0</v>
       </c>
       <c r="M12" s="5" t="s">
         <v>102</v>
@@ -3549,10 +3546,10 @@
         <v>0.5</v>
       </c>
       <c r="O12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -3577,7 +3574,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3877,7 +3874,7 @@
         <v>76</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>75</v>
@@ -3915,7 +3912,7 @@
         <v>76</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>75</v>
@@ -3938,7 +3935,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3976,7 +3973,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3991,7 +3988,7 @@
         <v>76</v>
       </c>
       <c r="F11">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>75</v>
@@ -4014,7 +4011,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4061,9 +4058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9730D4B9-BF36-445D-9853-EF3DA446843F}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A11" sqref="A11:R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4093,7 +4090,7 @@
         <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -4120,13 +4117,13 @@
         <v>68</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>19</v>
@@ -4135,7 +4132,7 @@
         <v>20</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -4252,7 +4249,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="16">
         <v>0</v>
@@ -4261,7 +4258,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>22</v>
@@ -4338,10 +4335,10 @@
         <v>0</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
@@ -4394,10 +4391,10 @@
         <v>0</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -4450,10 +4447,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M7" s="3">
         <v>0</v>
@@ -4506,10 +4503,10 @@
         <v>0</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
@@ -4562,10 +4559,10 @@
         <v>0</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L9" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
@@ -4618,10 +4615,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
@@ -4756,7 +4753,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -4812,7 +4809,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -4868,7 +4865,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -5036,7 +5033,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -5157,33 +5154,33 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="H2" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>58</v>
@@ -5198,91 +5195,91 @@
         <v>63</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="H4" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="H5" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="H6" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -5401,26 +5398,26 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" t="s">
         <v>138</v>
-      </c>
-      <c r="B12" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -5428,15 +5425,15 @@
         <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -5465,10 +5462,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" t="s">
         <v>112</v>
-      </c>
-      <c r="G1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -5485,7 +5482,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>69</v>
@@ -5508,31 +5505,31 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -5540,31 +5537,31 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -5572,31 +5569,31 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -5604,31 +5601,31 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -5636,31 +5633,31 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -5668,31 +5665,31 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -5700,31 +5697,31 @@
         <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -5732,31 +5729,31 @@
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -5764,31 +5761,31 @@
         <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -5796,31 +5793,31 @@
         <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -5828,31 +5825,31 @@
         <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -5874,7 +5871,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
adding separation processes as stand-alone intervals, DONE
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9AFD9F-954A-4C55-9EBB-46CFC107218C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7650BC8-9D6D-41ED-AD2F-3DBAA1C0D7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="167">
   <si>
     <t>components</t>
   </si>
@@ -368,9 +368,6 @@
   </si>
   <si>
     <t>cost_waste</t>
-  </si>
-  <si>
-    <t>€/kg</t>
   </si>
   <si>
     <t>lala et al (2022)</t>
@@ -541,12 +538,30 @@
   <si>
     <t>glu, fru, glycerol</t>
   </si>
+  <si>
+    <t>P_acidi</t>
+  </si>
+  <si>
+    <t>P_freu</t>
+  </si>
+  <si>
+    <t>P_avi</t>
+  </si>
+  <si>
+    <t>P_acn</t>
+  </si>
+  <si>
+    <t>P_pro</t>
+  </si>
+  <si>
+    <t>HHO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,13 +585,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -627,7 +649,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -787,7 +827,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -849,11 +889,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1074,13 +1123,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>34290</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>1172210</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>2540</xdr:rowOff>
@@ -1232,16 +1281,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>2286000</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>33020</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1231900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1256,8 +1305,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8663940" y="2383790"/>
-          <a:ext cx="2131060" cy="2221230"/>
+          <a:off x="20262850" y="222250"/>
+          <a:ext cx="1143000" cy="2870200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1531,15 +1580,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>353272</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>153880</xdr:rowOff>
+      <xdr:colOff>429472</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>84030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>233256</xdr:colOff>
+      <xdr:colOff>309456</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>23707</xdr:rowOff>
+      <xdr:rowOff>138007</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1554,8 +1603,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11387032" y="3262840"/>
-          <a:ext cx="2905124" cy="3710307"/>
+          <a:off x="11446722" y="3398730"/>
+          <a:ext cx="2889884" cy="3736977"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2663,7 +2712,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2764,7 +2813,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2779,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2856,18 +2905,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="5" width="17.26953125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" style="34" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
@@ -2875,31 +2925,30 @@
     <col min="10" max="10" width="16.36328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="41.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="D1" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>127</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>82</v>
@@ -2923,51 +2972,45 @@
         <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="S1" s="20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>8</v>
+        <v>161</v>
       </c>
       <c r="B2" s="5">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J2">
         <v>15</v>
@@ -2976,54 +3019,48 @@
         <v>95</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N2">
-        <v>0.5</v>
-      </c>
-      <c r="O2" t="s">
-        <v>109</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
-        <v>7</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G3">
         <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J3">
         <v>15</v>
@@ -3032,54 +3069,48 @@
         <v>95</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M3" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N3">
-        <v>0.5</v>
-      </c>
-      <c r="O3" t="s">
-        <v>109</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G4">
         <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J4">
         <v>15</v>
@@ -3088,54 +3119,48 @@
         <v>95</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M4" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N4">
-        <v>0.5</v>
-      </c>
-      <c r="O4" t="s">
-        <v>109</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
-        <v>10</v>
+        <v>164</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G5">
         <v>100</v>
       </c>
       <c r="H5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J5">
         <v>15</v>
@@ -3144,54 +3169,48 @@
         <v>95</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M5" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N5">
-        <v>0.5</v>
-      </c>
-      <c r="O5" t="s">
-        <v>109</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
-        <v>26</v>
+        <v>165</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G6">
         <v>100</v>
       </c>
       <c r="H6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J6">
         <v>15</v>
@@ -3200,28 +3219,22 @@
         <v>95</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M6" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N6">
-        <v>0.5</v>
-      </c>
-      <c r="O6" t="s">
-        <v>109</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>49</v>
       </c>
@@ -3229,25 +3242,25 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>131</v>
-      </c>
       <c r="F7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G7">
         <v>100</v>
       </c>
       <c r="H7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J7">
         <v>15</v>
@@ -3259,25 +3272,19 @@
         <v>54</v>
       </c>
       <c r="M7" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N7">
-        <v>0.5</v>
-      </c>
-      <c r="O7" t="s">
-        <v>109</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
         <v>67</v>
       </c>
@@ -3285,10 +3292,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" s="33">
         <v>0</v>
@@ -3300,7 +3307,7 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>98</v>
@@ -3314,26 +3321,20 @@
       <c r="L8" s="5">
         <v>0</v>
       </c>
-      <c r="M8" s="5">
-        <v>0</v>
+      <c r="M8" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="N8">
-        <v>0.5</v>
-      </c>
-      <c r="O8" t="s">
-        <v>109</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
         <v>68</v>
       </c>
@@ -3341,7 +3342,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>97</v>
@@ -3371,49 +3372,43 @@
       <c r="L9" s="5">
         <v>0</v>
       </c>
-      <c r="M9" s="5">
-        <v>0</v>
+      <c r="M9" s="5" t="s">
+        <v>153</v>
       </c>
       <c r="N9">
-        <v>0.5</v>
-      </c>
-      <c r="O9" t="s">
-        <v>109</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B10" s="33">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" s="33">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>89</v>
+      <c r="F10" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="42">
+        <v>3</v>
+      </c>
+      <c r="H10" s="42" t="s">
+        <v>119</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>104</v>
@@ -3428,36 +3423,30 @@
         <v>0</v>
       </c>
       <c r="M10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="N10">
-        <v>0.5</v>
-      </c>
-      <c r="O10" t="s">
-        <v>109</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11" s="33">
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="33">
         <v>0</v>
@@ -3484,36 +3473,30 @@
         <v>0</v>
       </c>
       <c r="M11" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q11" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="N11">
-        <v>0.5</v>
-      </c>
-      <c r="O11" t="s">
-        <v>109</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="S11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12" s="33">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E12" s="33">
         <v>0</v>
@@ -3540,26 +3523,17 @@
         <v>0</v>
       </c>
       <c r="M12" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="N12">
-        <v>0.5</v>
-      </c>
-      <c r="O12" t="s">
-        <v>109</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="N13" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3574,7 +3548,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3631,7 +3605,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>161</v>
       </c>
       <c r="B2">
         <v>1E-3</v>
@@ -3669,7 +3643,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>7</v>
+        <v>162</v>
       </c>
       <c r="B3">
         <v>1E-3</v>
@@ -3707,7 +3681,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="B4">
         <v>1E-3</v>
@@ -3745,7 +3719,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>164</v>
       </c>
       <c r="B5">
         <v>1E-3</v>
@@ -3783,7 +3757,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>165</v>
       </c>
       <c r="B6">
         <v>1E-3</v>
@@ -3935,7 +3909,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3973,7 +3947,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4011,7 +3985,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4058,9 +4032,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9730D4B9-BF36-445D-9853-EF3DA446843F}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A11" sqref="A11:R11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4090,24 +4064,24 @@
         <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" s="38" t="s">
         <v>49</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -4117,13 +4091,13 @@
         <v>68</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>19</v>
@@ -4132,11 +4106,11 @@
         <v>20</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="37" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -4192,7 +4166,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="37" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="16">
@@ -4248,8 +4222,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>114</v>
+      <c r="A4" s="37" t="s">
+        <v>113</v>
       </c>
       <c r="B4" s="16">
         <v>0</v>
@@ -4258,7 +4232,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>22</v>
@@ -4304,8 +4278,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
+      <c r="A5" s="38" t="s">
+        <v>161</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -4335,10 +4309,10 @@
         <v>0</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
@@ -4360,8 +4334,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
+      <c r="A6" s="38" t="s">
+        <v>162</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -4391,10 +4365,10 @@
         <v>0</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -4416,8 +4390,8 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>9</v>
+      <c r="A7" s="38" t="s">
+        <v>163</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -4447,10 +4421,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M7" s="3">
         <v>0</v>
@@ -4472,8 +4446,8 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>10</v>
+      <c r="A8" s="38" t="s">
+        <v>164</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -4503,10 +4477,10 @@
         <v>0</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
@@ -4528,8 +4502,8 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>26</v>
+      <c r="A9" s="38" t="s">
+        <v>165</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -4559,10 +4533,10 @@
         <v>0</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L9" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
@@ -4584,7 +4558,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="38" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="1">
@@ -4615,10 +4589,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
@@ -4640,7 +4614,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="1">
@@ -4670,7 +4644,7 @@
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="K11" s="37">
+      <c r="K11" s="1">
         <v>0</v>
       </c>
       <c r="L11" s="1">
@@ -4696,7 +4670,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="39" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="1">
@@ -4752,8 +4726,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>158</v>
+      <c r="A13" s="39" t="s">
+        <v>157</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -4808,8 +4782,8 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>159</v>
+      <c r="A14" s="39" t="s">
+        <v>158</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -4864,8 +4838,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>160</v>
+      <c r="A15" s="39" t="s">
+        <v>159</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -4920,7 +4894,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="40" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1">
@@ -4976,7 +4950,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="40" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="1">
@@ -5032,8 +5006,8 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>118</v>
+      <c r="A18" s="41" t="s">
+        <v>117</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -5089,7 +5063,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B16:J17 B5:D15 K2:R10 B18:R18 E2:J15 K12:R17 L11:R11">
+  <conditionalFormatting sqref="B16:J17 B5:D15 B18:R18 E2:J15 K2:R17">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -5154,33 +5128,33 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>148</v>
-      </c>
       <c r="H2" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>58</v>
@@ -5195,91 +5169,91 @@
         <v>63</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>148</v>
-      </c>
       <c r="H4" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>148</v>
-      </c>
       <c r="H5" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>148</v>
-      </c>
       <c r="H6" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -5398,26 +5372,26 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" t="s">
         <v>137</v>
-      </c>
-      <c r="B12" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -5425,15 +5399,15 @@
         <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5462,10 +5436,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
         <v>111</v>
-      </c>
-      <c r="G1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -5505,31 +5479,31 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -5537,31 +5511,31 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -5569,31 +5543,31 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -5601,31 +5575,31 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -5633,31 +5607,31 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -5665,31 +5639,31 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -5697,31 +5671,31 @@
         <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -5729,31 +5703,31 @@
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -5761,31 +5735,31 @@
         <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -5793,31 +5767,31 @@
         <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -5825,31 +5799,31 @@
         <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -5871,7 +5845,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
adding function to make boolean equations
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DFD998-1A9D-4F62-A159-1A5E4D7FA34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38D49C8-8264-47EC-83A9-E7F5CB143B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" firstSheet="2" activeTab="4" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
     <sheet name="process_intervals" sheetId="18" r:id="rId2"/>
     <sheet name="economic_parameters" sheetId="17" r:id="rId3"/>
     <sheet name="connection_matrix" sheetId="11" r:id="rId4"/>
-    <sheet name="models" sheetId="14" r:id="rId5"/>
-    <sheet name="abbr" sheetId="15" r:id="rId6"/>
-    <sheet name="references" sheetId="19" r:id="rId7"/>
-    <sheet name="calculations" sheetId="20" r:id="rId8"/>
+    <sheet name="connection_matrix_test" sheetId="21" r:id="rId5"/>
+    <sheet name="models" sheetId="14" r:id="rId6"/>
+    <sheet name="abbr" sheetId="15" r:id="rId7"/>
+    <sheet name="references" sheetId="19" r:id="rId8"/>
+    <sheet name="calculations" sheetId="20" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="182">
   <si>
     <t>components</t>
   </si>
@@ -567,6 +568,39 @@
   </si>
   <si>
     <t>{'temp':[25,80]}</t>
+  </si>
+  <si>
+    <t>porp</t>
+  </si>
+  <si>
+    <t>serpa1</t>
+  </si>
+  <si>
+    <t>serpa2</t>
+  </si>
+  <si>
+    <t>y_acidi</t>
+  </si>
+  <si>
+    <t>y_frue</t>
+  </si>
+  <si>
+    <t>y_avi</t>
+  </si>
+  <si>
+    <t>y_acn</t>
+  </si>
+  <si>
+    <t>y_pro</t>
+  </si>
+  <si>
+    <t>y_open</t>
+  </si>
+  <si>
+    <t>y_liq_liq</t>
+  </si>
+  <si>
+    <t>y_NF</t>
   </si>
 </sst>
 </file>
@@ -839,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -916,6 +950,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1955,6 +1993,280 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>429472</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>84030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>309456</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>138007</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{929A0913-D5E0-4497-BD47-A7934C84045D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11446722" y="3398730"/>
+          <a:ext cx="2889884" cy="3736977"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100"/>
+            <a:t>connect by looking</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t> at which streams connect to the next intervall (i.e wat are the reactor inputs and how are they connected to their outputs)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>0 -&gt; not connencted </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>1 -&gt; connected </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>mix in the same colunm indiacte that the outputs of the intervals are mixed</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>sep_nr = define which seperation stream goes where</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>split_nr = define which split stream goes where</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>options :</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>bool, split, sep 0 or  1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>can be a combination </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>700404</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22224</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>413596</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>138430</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95B6E699-CD2D-4A38-88BF-4D9197B5C743}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1856104" y="3336924"/>
+          <a:ext cx="3783542" cy="1957706"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>green matrix: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>say from the all the posible substrate or from a subset of them, you only want to select one possibilty! you can by definbing the boolean variable in the diagonal of the green matix. in this case only one carbon source can be choosen because the equation y1 + y2 == 1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>for a more complicated example see test_area </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>548639</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>61134</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>251060</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{629B3289-EFEB-4A7A-B778-1BC14A780257}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5774689" y="3375834"/>
+          <a:ext cx="5493621" cy="2301066"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>142240</xdr:colOff>
       <xdr:row>8</xdr:row>
@@ -2428,7 +2740,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3009,7 +3321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="I16" sqref="I16"/>
     </sheetView>
@@ -4213,7 +4525,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N13" sqref="N13"/>
+      <selection pane="topRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5259,12 +5571,1063 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B92B1C5-379D-4587-B23B-6C3AF487A07D}">
+  <dimension ref="A1:R18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="15">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1</v>
+      </c>
+      <c r="J4" s="15">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="M12" s="32">
+        <v>0</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="32">
+        <v>0</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="32">
+        <v>0</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B18:R18 E2:J4 B5:J17 K2:R17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8D8FB7-0FD2-42C3-9D82-0A6D9AE32488}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J6" sqref="J6"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5467,7 +6830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFEA29F-1D3A-4383-97E1-D31836BA3887}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -5594,7 +6957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE819A9C-4E64-4D0F-8F31-2F1BF4DCFD79}">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -6012,22 +7375,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5E6B06-BC4E-40C6-BE72-7273BEB1C476}">
-  <dimension ref="B2:G15"/>
+  <dimension ref="B2:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="15.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B3" s="24"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
@@ -6039,7 +7405,7 @@
       </c>
       <c r="G3" s="26"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B4" s="27"/>
       <c r="E4">
         <f>E3*10^-3</f>
@@ -6049,12 +7415,60 @@
         <v>85</v>
       </c>
       <c r="G4" s="28"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="N4" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="O4" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="P4" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q4" s="44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" s="27"/>
       <c r="G5" s="28"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J5" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="16">
+        <v>0</v>
+      </c>
+      <c r="M5" s="16">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>1</v>
+      </c>
+      <c r="O5" s="6">
+        <v>1</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B6" s="27"/>
       <c r="C6" t="s">
         <v>86</v>
@@ -6063,12 +7477,60 @@
         <v>87</v>
       </c>
       <c r="G6" s="28"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J6" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="16">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>1</v>
+      </c>
+      <c r="O6" s="6">
+        <v>1</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B7" s="27"/>
       <c r="G7" s="28"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J7" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="N7" s="10">
+        <v>1</v>
+      </c>
+      <c r="O7" s="10">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B8" s="27"/>
       <c r="C8">
         <v>100</v>
@@ -6087,8 +7549,32 @@
         <f>E8/C8</f>
         <v>66.666666666666671</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J8" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0</v>
+      </c>
+      <c r="P8" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q8" s="45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" s="27"/>
       <c r="C9">
         <v>150</v>
@@ -6107,8 +7593,32 @@
         <f>E9/C9</f>
         <v>66.666666666666671</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J9" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="P9" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q9" s="45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B10" s="27">
         <v>200</v>
       </c>
@@ -6127,8 +7637,32 @@
         <v>66.666666666666671</v>
       </c>
       <c r="G10" s="28"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J10" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B11" s="27">
         <v>250</v>
       </c>
@@ -6147,8 +7681,32 @@
         <v>66.666666666666671</v>
       </c>
       <c r="G11" s="28"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J11" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B12" s="27">
         <v>300</v>
       </c>
@@ -6168,7 +7726,7 @@
       </c>
       <c r="G12" s="28"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B13" s="27">
         <v>350</v>
       </c>
@@ -6188,7 +7746,7 @@
       </c>
       <c r="G13" s="28"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B14" s="27">
         <v>400</v>
       </c>
@@ -6208,7 +7766,7 @@
       </c>
       <c r="G14" s="28"/>
     </row>
-    <row r="15" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="29">
         <v>450</v>
       </c>
@@ -6229,6 +7787,17 @@
       <c r="G15" s="31"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="N5:N8 O9 O5:O7">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding cost model (GREV and OPEX)
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9522715E-20D9-492B-A2FE-28AB170BC0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05C3429-BF46-477D-82F5-8B890EF9D19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" firstSheet="1" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="234">
   <si>
     <t>components</t>
   </si>
@@ -731,9 +731,6 @@
     <t>discription</t>
   </si>
   <si>
-    <t>testDistilation.json</t>
-  </si>
-  <si>
     <t>{'x_D':0,95,}</t>
   </si>
   <si>
@@ -741,6 +738,27 @@
   </si>
   <si>
     <t>kWh/kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DWA </t>
+  </si>
+  <si>
+    <t>McCubbin et al</t>
+  </si>
+  <si>
+    <t>Patent mateo</t>
+  </si>
+  <si>
+    <t>TOFIND</t>
+  </si>
+  <si>
+    <t>Koyuncu et al (2000)</t>
+  </si>
+  <si>
+    <t>processing principles book</t>
+  </si>
+  <si>
+    <t>Reguiera et al (2018)</t>
   </si>
 </sst>
 </file>
@@ -5443,8 +5461,8 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P11" sqref="P11"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5462,7 +5480,7 @@
     <col min="12" max="12" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.36328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.26953125" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="41.1796875" bestFit="1" customWidth="1"/>
@@ -5522,7 +5540,7 @@
         <v>177</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>74</v>
@@ -5590,10 +5608,11 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <f xml:space="preserve"> 0.5*0.001</f>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>115</v>
@@ -5658,10 +5677,11 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <f t="shared" ref="P3:P7" si="0" xml:space="preserve"> 0.5*0.001</f>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>116</v>
@@ -5726,10 +5746,11 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>117</v>
@@ -5794,10 +5815,11 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>118</v>
@@ -5862,10 +5884,11 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>119</v>
@@ -5930,10 +5953,11 @@
         <v>178</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>54</v>
@@ -5998,10 +6022,10 @@
         <v>178</v>
       </c>
       <c r="P8">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="Q8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R8" s="5">
         <v>0</v>
@@ -6066,10 +6090,11 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>10</v>
+        <f>2.5*10^(-3)</f>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="Q9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R9" s="5">
         <v>0</v>
@@ -6128,16 +6153,16 @@
         <v>0</v>
       </c>
       <c r="N10" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O10" s="5" t="s">
         <v>221</v>
       </c>
       <c r="P10">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="Q10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R10" s="5">
         <v>0</v>
@@ -6201,11 +6226,11 @@
       <c r="O11" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="P11" t="s">
-        <v>224</v>
+      <c r="P11">
+        <v>0.1</v>
       </c>
       <c r="Q11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R11" s="5">
         <v>0</v>
@@ -6270,10 +6295,10 @@
         <v>221</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0.08</v>
       </c>
       <c r="Q12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R12" s="5">
         <v>0</v>
@@ -6304,7 +6329,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6360,7 +6385,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="22" t="s">
         <v>154</v>
       </c>
       <c r="B2">
@@ -6398,7 +6423,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="22" t="s">
         <v>155</v>
       </c>
       <c r="B3">
@@ -6436,7 +6461,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="22" t="s">
         <v>156</v>
       </c>
       <c r="B4">
@@ -6474,7 +6499,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="22" t="s">
         <v>157</v>
       </c>
       <c r="B5">
@@ -6512,7 +6537,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="22" t="s">
         <v>158</v>
       </c>
       <c r="B6">
@@ -6550,7 +6575,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B7">
@@ -6588,7 +6613,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="21" t="s">
         <v>67</v>
       </c>
       <c r="B8">
@@ -6626,7 +6651,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B9">
@@ -6664,7 +6689,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="21" t="s">
         <v>150</v>
       </c>
       <c r="B10">
@@ -6702,7 +6727,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="21" t="s">
         <v>151</v>
       </c>
       <c r="B11">
@@ -6740,7 +6765,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="21" t="s">
         <v>152</v>
       </c>
       <c r="B12">
@@ -8266,7 +8291,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8546,14 +8571,14 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.90625" customWidth="1"/>
     <col min="8" max="8" width="17.26953125" customWidth="1"/>
@@ -8604,14 +8629,14 @@
       <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" t="s">
-        <v>104</v>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>228</v>
       </c>
       <c r="E4" t="s">
         <v>104</v>
@@ -8636,14 +8661,14 @@
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" t="s">
-        <v>104</v>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>228</v>
       </c>
       <c r="E5" t="s">
         <v>104</v>
@@ -8668,14 +8693,14 @@
       <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" t="s">
-        <v>104</v>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>228</v>
       </c>
       <c r="E6" t="s">
         <v>104</v>
@@ -8700,14 +8725,14 @@
       <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" t="s">
-        <v>104</v>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>228</v>
       </c>
       <c r="E7" t="s">
         <v>104</v>
@@ -8732,14 +8757,14 @@
       <c r="A8" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" t="s">
-        <v>104</v>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>228</v>
       </c>
       <c r="E8" t="s">
         <v>104</v>
@@ -8764,14 +8789,14 @@
       <c r="A9" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" t="s">
-        <v>104</v>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>233</v>
       </c>
       <c r="E9" t="s">
         <v>104</v>
@@ -8797,13 +8822,10 @@
         <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" t="s">
-        <v>104</v>
+        <v>229</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>230</v>
       </c>
       <c r="E10" t="s">
         <v>104</v>
@@ -8828,14 +8850,11 @@
       <c r="A11" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" t="s">
-        <v>104</v>
+      <c r="B11" s="39">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="E11" t="s">
         <v>104</v>
@@ -8861,13 +8880,10 @@
         <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" t="s">
-        <v>104</v>
+        <v>229</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="E12" t="s">
         <v>104</v>
@@ -8893,13 +8909,10 @@
         <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" t="s">
-        <v>104</v>
+        <v>229</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="E13" t="s">
         <v>104</v>
@@ -8925,13 +8938,10 @@
         <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" t="s">
-        <v>104</v>
+        <v>229</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="E14" t="s">
         <v>104</v>
@@ -8955,6 +8965,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cost model working + fixes to open-fermentation ml model
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05C3429-BF46-477D-82F5-8B890EF9D19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499CDA28-032B-41BA-A86F-E2147C8013A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" firstSheet="1" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -1088,7 +1088,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1126,6 +1125,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1349,8 +1349,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1366,7 +1366,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7708900" y="1854200"/>
-          <a:ext cx="2286000" cy="520700"/>
+          <a:ext cx="2286000" cy="1231900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1440,6 +1440,27 @@
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
             <a:t> 0.39 €/kg</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>price acetate: 1.15 euro/kg</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>price propionate: 1.26 euro/kg</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2465,15 +2486,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>618489</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>16684</xdr:rowOff>
+      <xdr:colOff>486953</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>98326</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>320910</xdr:colOff>
+      <xdr:colOff>189374</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>3628</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2496,8 +2517,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5844539" y="3515534"/>
-          <a:ext cx="5493621" cy="2301066"/>
+          <a:off x="5712096" y="3445683"/>
+          <a:ext cx="5489992" cy="2322838"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3787,7 +3808,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3839,13 +3860,13 @@
         <v>56</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="E2">
-        <v>0.2</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -3865,10 +3886,10 @@
         <v>57</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="E3">
         <v>0.39</v>
@@ -3891,13 +3912,13 @@
         <v>108</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D4">
-        <v>1000</v>
-      </c>
-      <c r="E4" s="23">
-        <v>0.4</v>
+        <v>10000</v>
+      </c>
+      <c r="E4">
+        <v>0.35</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -3926,7 +3947,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1.1499999999999999</v>
+        <v>2.5</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>17</v>
@@ -3952,7 +3973,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1.26</v>
+        <v>5</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>16</v>
@@ -3997,19 +4018,19 @@
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25">
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24">
         <v>15</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="26"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B4" s="27"/>
+      <c r="B4" s="26"/>
       <c r="E4">
         <f>E3*10^-3</f>
         <v>1.4999999999999999E-2</v>
@@ -4017,36 +4038,36 @@
       <c r="F4" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="27"/>
       <c r="J4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="34" t="s">
+      <c r="K4" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="L4" s="34" t="s">
+      <c r="L4" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="34" t="s">
+      <c r="M4" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="N4" s="35" t="s">
+      <c r="N4" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="O4" s="35" t="s">
+      <c r="O4" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="P4" s="41" t="s">
+      <c r="P4" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="Q4" s="41" t="s">
+      <c r="Q4" s="40" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B5" s="27"/>
-      <c r="G5" s="28"/>
-      <c r="J5" s="34" t="s">
+      <c r="B5" s="26"/>
+      <c r="G5" s="27"/>
+      <c r="J5" s="33" t="s">
         <v>56</v>
       </c>
       <c r="K5" s="16" t="s">
@@ -4072,15 +4093,15 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B6" s="27"/>
+      <c r="B6" s="26"/>
       <c r="C6" t="s">
         <v>86</v>
       </c>
       <c r="E6" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="J6" s="34" t="s">
+      <c r="G6" s="27"/>
+      <c r="J6" s="33" t="s">
         <v>57</v>
       </c>
       <c r="K6" s="16">
@@ -4106,9 +4127,9 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B7" s="27"/>
-      <c r="G7" s="28"/>
-      <c r="J7" s="34" t="s">
+      <c r="B7" s="26"/>
+      <c r="G7" s="27"/>
+      <c r="J7" s="33" t="s">
         <v>108</v>
       </c>
       <c r="K7" s="16">
@@ -4134,7 +4155,7 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B8" s="27"/>
+      <c r="B8" s="26"/>
       <c r="C8">
         <v>100</v>
       </c>
@@ -4148,11 +4169,11 @@
       <c r="F8" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="27">
         <f>E8/C8</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="34" t="s">
         <v>154</v>
       </c>
       <c r="K8" s="5">
@@ -4170,15 +4191,15 @@
       <c r="O8" s="5">
         <v>0</v>
       </c>
-      <c r="P8" s="42" t="s">
+      <c r="P8" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="Q8" s="42" t="s">
+      <c r="Q8" s="41" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B9" s="27"/>
+      <c r="B9" s="26"/>
       <c r="C9">
         <v>150</v>
       </c>
@@ -4192,11 +4213,11 @@
       <c r="F9" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="27">
         <f>E9/C9</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="34" t="s">
         <v>155</v>
       </c>
       <c r="K9" s="5">
@@ -4214,15 +4235,15 @@
       <c r="O9" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="P9" s="42" t="s">
+      <c r="P9" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="Q9" s="42" t="s">
+      <c r="Q9" s="41" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B10" s="27">
+      <c r="B10" s="26">
         <v>200</v>
       </c>
       <c r="C10" t="s">
@@ -4239,8 +4260,8 @@
         <f t="shared" ref="F10:F15" si="1">D10/B10</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="J10" s="41" t="s">
+      <c r="G10" s="27"/>
+      <c r="J10" s="40" t="s">
         <v>161</v>
       </c>
       <c r="K10" s="5">
@@ -4266,7 +4287,7 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B11" s="27">
+      <c r="B11" s="26">
         <v>250</v>
       </c>
       <c r="C11" t="s">
@@ -4283,8 +4304,8 @@
         <f t="shared" si="1"/>
         <v>66.666666666666671</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="J11" s="41" t="s">
+      <c r="G11" s="27"/>
+      <c r="J11" s="40" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="5">
@@ -4310,7 +4331,7 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B12" s="27">
+      <c r="B12" s="26">
         <v>300</v>
       </c>
       <c r="C12" t="s">
@@ -4327,10 +4348,10 @@
         <f t="shared" si="1"/>
         <v>66.666666666666671</v>
       </c>
-      <c r="G12" s="28"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B13" s="27">
+      <c r="B13" s="26">
         <v>350</v>
       </c>
       <c r="C13" t="s">
@@ -4347,10 +4368,10 @@
         <f t="shared" si="1"/>
         <v>66.666666666666671</v>
       </c>
-      <c r="G13" s="28"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B14" s="27">
+      <c r="B14" s="26">
         <v>400</v>
       </c>
       <c r="C14" t="s">
@@ -4367,27 +4388,27 @@
         <f t="shared" si="1"/>
         <v>66.666666666666671</v>
       </c>
-      <c r="G14" s="28"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="29">
+      <c r="B15" s="28">
         <v>450</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="29">
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="29">
         <f t="shared" si="1"/>
         <v>66.666666666666671</v>
       </c>
-      <c r="G15" s="31"/>
+      <c r="G15" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4443,22 +4464,22 @@
       <c r="D1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="34" t="s">
         <v>49</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -4487,7 +4508,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -4543,7 +4564,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="16">
@@ -4599,7 +4620,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>108</v>
       </c>
       <c r="B4" s="16">
@@ -4655,7 +4676,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>154</v>
       </c>
       <c r="B5" s="1">
@@ -4711,7 +4732,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>155</v>
       </c>
       <c r="B6" s="1">
@@ -4767,7 +4788,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="34" t="s">
         <v>156</v>
       </c>
       <c r="B7" s="1">
@@ -4823,7 +4844,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>157</v>
       </c>
       <c r="B8" s="1">
@@ -4879,7 +4900,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="34" t="s">
         <v>158</v>
       </c>
       <c r="B9" s="1">
@@ -4935,7 +4956,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="34" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="1">
@@ -4991,7 +5012,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="1">
@@ -5047,7 +5068,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="1">
@@ -5103,7 +5124,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>150</v>
       </c>
       <c r="B13" s="1">
@@ -5159,7 +5180,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="35" t="s">
         <v>151</v>
       </c>
       <c r="B14" s="1">
@@ -5215,7 +5236,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>152</v>
       </c>
       <c r="B15" s="1">
@@ -5271,7 +5292,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1">
@@ -5327,7 +5348,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="1">
@@ -5383,7 +5404,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="37" t="s">
         <v>112</v>
       </c>
       <c r="B18" s="1">
@@ -5460,9 +5481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P4" sqref="P4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5474,7 +5495,7 @@
     <col min="6" max="6" width="17.26953125" customWidth="1"/>
     <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="4.90625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.08984375" bestFit="1" customWidth="1"/>
@@ -5598,10 +5619,10 @@
       <c r="L2" s="5">
         <v>0</v>
       </c>
-      <c r="M2" s="32">
-        <v>0</v>
-      </c>
-      <c r="N2" s="32">
+      <c r="M2" s="31">
+        <v>0</v>
+      </c>
+      <c r="N2" s="31">
         <v>0</v>
       </c>
       <c r="O2" s="5">
@@ -5922,7 +5943,7 @@
       <c r="E7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="31">
         <v>0</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -5934,22 +5955,22 @@
       <c r="I7" t="s">
         <v>114</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="39" t="s">
         <v>142</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="L7" s="32" t="s">
+      <c r="L7" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="N7" s="32" t="s">
+      <c r="N7" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="O7" s="32" t="s">
+      <c r="O7" s="31" t="s">
         <v>178</v>
       </c>
       <c r="P7">
@@ -6015,10 +6036,10 @@
       <c r="M8" s="5">
         <v>0</v>
       </c>
-      <c r="N8" s="32">
-        <v>0</v>
-      </c>
-      <c r="O8" s="32" t="s">
+      <c r="N8" s="31">
+        <v>0</v>
+      </c>
+      <c r="O8" s="31" t="s">
         <v>178</v>
       </c>
       <c r="P8">
@@ -6083,10 +6104,10 @@
       <c r="M9" s="5">
         <v>0</v>
       </c>
-      <c r="N9" s="32">
-        <v>0</v>
-      </c>
-      <c r="O9" s="32">
+      <c r="N9" s="31">
+        <v>0</v>
+      </c>
+      <c r="O9" s="31">
         <v>0</v>
       </c>
       <c r="P9">
@@ -6134,7 +6155,7 @@
       <c r="G10" s="5">
         <v>0</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="38">
         <v>0</v>
       </c>
       <c r="I10" t="s">
@@ -6152,7 +6173,7 @@
       <c r="M10" s="5">
         <v>0</v>
       </c>
-      <c r="N10" s="32" t="s">
+      <c r="N10" s="31" t="s">
         <v>224</v>
       </c>
       <c r="O10" s="5" t="s">
@@ -6220,10 +6241,10 @@
       <c r="M11" s="5">
         <v>0</v>
       </c>
-      <c r="N11" s="32" t="s">
+      <c r="N11" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="O11" s="32" t="s">
+      <c r="O11" s="31" t="s">
         <v>221</v>
       </c>
       <c r="P11">
@@ -6288,10 +6309,10 @@
       <c r="M12" s="5">
         <v>0</v>
       </c>
-      <c r="N12" s="32" t="s">
+      <c r="N12" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="O12" s="32" t="s">
+      <c r="O12" s="31" t="s">
         <v>221</v>
       </c>
       <c r="P12">
@@ -6329,7 +6350,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6400,8 +6421,8 @@
       <c r="E2" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F2">
-        <v>2E-3</v>
+      <c r="F2" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>75</v>
@@ -6438,8 +6459,8 @@
       <c r="E3" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F3">
-        <v>2E-3</v>
+      <c r="F3" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>75</v>
@@ -6476,8 +6497,8 @@
       <c r="E4" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F4">
-        <v>2E-3</v>
+      <c r="F4" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>75</v>
@@ -6514,8 +6535,8 @@
       <c r="E5" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F5">
-        <v>2E-3</v>
+      <c r="F5" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>75</v>
@@ -6552,8 +6573,8 @@
       <c r="E6" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F6">
-        <v>2E-3</v>
+      <c r="F6" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>75</v>
@@ -6590,8 +6611,8 @@
       <c r="E7" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F7">
-        <v>2E-3</v>
+      <c r="F7" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>75</v>
@@ -6628,8 +6649,8 @@
       <c r="E8" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F8">
-        <v>2E-3</v>
+      <c r="F8" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>75</v>
@@ -6666,8 +6687,8 @@
       <c r="E9" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F9">
-        <v>2E-3</v>
+      <c r="F9" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>75</v>
@@ -6704,8 +6725,8 @@
       <c r="E10" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F10">
-        <v>5.0000000000000001E-3</v>
+      <c r="F10" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>75</v>
@@ -6742,8 +6763,8 @@
       <c r="E11" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F11">
-        <v>0</v>
+      <c r="F11" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>75</v>
@@ -6780,8 +6801,8 @@
       <c r="E12" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F12">
-        <v>5.0000000000000001E-3</v>
+      <c r="F12" s="46">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>75</v>
@@ -6813,9 +6834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B92B1C5-379D-4587-B23B-6C3AF487A07D}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E9" sqref="E9"/>
+      <selection pane="topRight" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6847,22 +6868,22 @@
       <c r="D1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="34" t="s">
         <v>49</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -6891,7 +6912,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -6947,7 +6968,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="16">
@@ -7003,7 +7024,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>108</v>
       </c>
       <c r="B4" s="16">
@@ -7059,7 +7080,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>154</v>
       </c>
       <c r="B5" s="1">
@@ -7115,7 +7136,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>155</v>
       </c>
       <c r="B6" s="1">
@@ -7171,7 +7192,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="34" t="s">
         <v>156</v>
       </c>
       <c r="B7" s="1">
@@ -7227,7 +7248,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>157</v>
       </c>
       <c r="B8" s="1">
@@ -7283,7 +7304,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="34" t="s">
         <v>158</v>
       </c>
       <c r="B9" s="1">
@@ -7339,7 +7360,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="34" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="1">
@@ -7395,7 +7416,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="1">
@@ -7451,7 +7472,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="1">
@@ -7507,7 +7528,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>150</v>
       </c>
       <c r="B13" s="1">
@@ -7563,7 +7584,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="35" t="s">
         <v>151</v>
       </c>
       <c r="B14" s="1">
@@ -7619,7 +7640,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>152</v>
       </c>
       <c r="B15" s="1">
@@ -7675,7 +7696,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1">
@@ -7731,7 +7752,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="1">
@@ -7787,7 +7808,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="37" t="s">
         <v>112</v>
       </c>
       <c r="B18" s="1">
@@ -8038,7 +8059,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="13">
@@ -8064,7 +8085,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>183</v>
       </c>
       <c r="B8" s="13"/>
@@ -8141,54 +8162,54 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2" s="44">
         <v>0.95</v>
       </c>
-      <c r="E2" s="45">
+      <c r="E2" s="44">
         <v>0.05</v>
       </c>
-      <c r="F2" s="46">
+      <c r="F2" s="45">
         <f xml:space="preserve"> 25 +273</f>
         <v>298</v>
       </c>
-      <c r="G2" s="46">
+      <c r="G2" s="45">
         <f>90 + 273</f>
         <v>363</v>
       </c>
-      <c r="H2" s="46">
+      <c r="H2" s="45">
         <f>125 + 273</f>
         <v>398</v>
       </c>
-      <c r="I2" s="46">
+      <c r="I2" s="45">
         <v>0.18</v>
       </c>
-      <c r="J2" s="46">
+      <c r="J2" s="45">
         <v>0.5</v>
       </c>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="L2" s="46" t="s">
+      <c r="L2" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="M2" s="46">
+      <c r="M2" s="45">
         <v>100</v>
       </c>
-      <c r="N2" s="46">
+      <c r="N2" s="45">
         <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>213</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -8203,39 +8224,39 @@
       <c r="E3" s="14">
         <v>0.05</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <f t="shared" ref="F3:F4" si="0" xml:space="preserve"> 25 +273</f>
         <v>298</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="45">
         <f t="shared" ref="G3:G4" si="1">90 + 273</f>
         <v>363</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <f t="shared" ref="H3:H4" si="2">125 + 273</f>
         <v>398</v>
       </c>
-      <c r="I3" s="46">
+      <c r="I3" s="45">
         <v>0.18</v>
       </c>
-      <c r="J3" s="46">
+      <c r="J3" s="45">
         <v>0.5</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="M3" s="46">
+      <c r="M3" s="45">
         <v>100</v>
       </c>
-      <c r="N3" s="46">
+      <c r="N3" s="45">
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="42" t="s">
         <v>214</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -8250,34 +8271,34 @@
       <c r="E4" s="14">
         <v>0.05</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <f t="shared" si="0"/>
         <v>298</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <f t="shared" si="1"/>
         <v>363</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <f t="shared" si="2"/>
         <v>398</v>
       </c>
-      <c r="I4" s="46">
+      <c r="I4" s="45">
         <v>0.18</v>
       </c>
-      <c r="J4" s="46">
+      <c r="J4" s="45">
         <v>0.5</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="L4" s="46" t="s">
+      <c r="L4" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="46">
+      <c r="M4" s="45">
         <v>100</v>
       </c>
-      <c r="N4" s="46">
+      <c r="N4" s="45">
         <v>80</v>
       </c>
     </row>
@@ -8824,7 +8845,7 @@
       <c r="B10" t="s">
         <v>229</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="39" t="s">
         <v>230</v>
       </c>
       <c r="E10" t="s">
@@ -8850,7 +8871,7 @@
       <c r="A11" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="38">
         <v>0</v>
       </c>
       <c r="C11" s="5" t="s">

</xml_diff>

<commit_message>
fixes to open-fermentation ml model
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499CDA28-032B-41BA-A86F-E2147C8013A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC772A2E-0922-44B8-A33E-1A0C7A1F3F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -187,12 +187,6 @@
     <t>pH</t>
   </si>
   <si>
-    <t>prop, ace</t>
-  </si>
-  <si>
-    <t>Propionate, Acetate</t>
-  </si>
-  <si>
     <t>open_fermentation</t>
   </si>
   <si>
@@ -206,9 +200,6 @@
   </si>
   <si>
     <t>fru</t>
-  </si>
-  <si>
-    <t>open_fermentation_polynomial_ESCAPE33.json</t>
   </si>
   <si>
     <t>fructose</t>
@@ -760,12 +751,42 @@
   <si>
     <t>Reguiera et al (2018)</t>
   </si>
+  <si>
+    <t>open_fermentation_polynomial_case_study.json</t>
+  </si>
+  <si>
+    <r>
+      <t>CV_Acetate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF000000"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF008000"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> CV_Propionate, CV_Biomass</t>
+    </r>
+  </si>
+  <si>
+    <t>ace, prop, bm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -800,6 +821,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF008000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1040,7 +1074,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1126,6 +1160,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2058,8 +2096,8 @@
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
@@ -2076,8 +2114,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15537180" y="2622550"/>
-          <a:ext cx="1766570" cy="723900"/>
+          <a:off x="15695930" y="2622550"/>
+          <a:ext cx="1684020" cy="723900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2839,15 +2877,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1159510</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>172720</xdr:rowOff>
+      <xdr:colOff>1131288</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>179775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1019810</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>39370</xdr:rowOff>
+      <xdr:colOff>991588</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>46426</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2862,8 +2900,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10760710" y="1452880"/>
-          <a:ext cx="4798060" cy="1329690"/>
+          <a:off x="10536344" y="2197664"/>
+          <a:ext cx="4785077" cy="1334206"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2946,15 +2984,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>261620</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>71120</xdr:rowOff>
+      <xdr:colOff>148731</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>162842</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1399540</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>151130</xdr:rowOff>
+      <xdr:colOff>1286651</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>59408</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2969,8 +3007,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11188700" y="2997200"/>
-          <a:ext cx="4749800" cy="3188970"/>
+          <a:off x="10880231" y="3831731"/>
+          <a:ext cx="4736253" cy="3198566"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3811,7 +3849,7 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -3826,7 +3864,7 @@
     <col min="12" max="12" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3852,12 +3890,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>10000</v>
@@ -3878,12 +3916,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="8">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>10000</v>
@@ -3898,18 +3936,18 @@
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="8">
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C4">
         <v>10000</v>
@@ -3924,13 +3962,13 @@
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="9">
         <v>7</v>
       </c>
@@ -3956,7 +3994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8">
       <c r="A6" s="9">
         <v>7</v>
       </c>
@@ -3982,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="D7" s="4"/>
       <c r="G7" s="4"/>
     </row>
@@ -4007,17 +4045,17 @@
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="10" max="10" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:17" ht="15" thickBot="1">
       <c r="B2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17">
       <c r="B3" s="23"/>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -4025,53 +4063,53 @@
         <v>15</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G3" s="25"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:17">
       <c r="B4" s="26"/>
       <c r="E4">
         <f>E3*10^-3</f>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G4" s="27"/>
       <c r="J4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N4" s="34" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="O4" s="34" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="Q4" s="40" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:17">
       <c r="B5" s="26"/>
       <c r="G5" s="27"/>
       <c r="J5" s="33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L5" s="16">
         <v>0</v>
@@ -4092,23 +4130,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:17">
       <c r="B6" s="26"/>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G6" s="27"/>
       <c r="J6" s="33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K6" s="16">
         <v>0</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M6" s="16">
         <v>0</v>
@@ -4126,11 +4164,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:17">
       <c r="B7" s="26"/>
       <c r="G7" s="27"/>
       <c r="J7" s="33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K7" s="16">
         <v>0</v>
@@ -4139,7 +4177,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N7" s="10">
         <v>1</v>
@@ -4154,27 +4192,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:17">
       <c r="B8" s="26"/>
       <c r="C8">
         <v>100</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E8">
         <f>C8/$E$4</f>
         <v>6666.666666666667</v>
       </c>
       <c r="F8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G8" s="27">
         <f>E8/C8</f>
         <v>66.666666666666671</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K8" s="5">
         <v>0</v>
@@ -4186,39 +4224,39 @@
         <v>0</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O8" s="5">
         <v>0</v>
       </c>
       <c r="P8" s="41" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="Q8" s="41" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17">
       <c r="B9" s="26"/>
       <c r="C9">
         <v>150</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E9">
         <f>C9/$E$4</f>
         <v>10000</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G9" s="27">
         <f>E9/C9</f>
         <v>66.666666666666671</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K9" s="5">
         <v>0</v>
@@ -4233,28 +4271,28 @@
         <v>0</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P9" s="41" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="Q9" s="41" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
       <c r="B10" s="26">
         <v>200</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D10">
         <f t="shared" ref="D10:D15" si="0">B10/$E$4</f>
         <v>13333.333333333334</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F10">
         <f t="shared" ref="F10:F15" si="1">D10/B10</f>
@@ -4262,7 +4300,7 @@
       </c>
       <c r="G10" s="27"/>
       <c r="J10" s="40" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K10" s="5">
         <v>0</v>
@@ -4286,19 +4324,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:17">
       <c r="B11" s="26">
         <v>250</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
         <v>16666.666666666668</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
@@ -4330,19 +4368,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17">
       <c r="B12" s="26">
         <v>300</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
@@ -4350,19 +4388,19 @@
       </c>
       <c r="G12" s="27"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:17">
       <c r="B13" s="26">
         <v>350</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
         <v>23333.333333333336</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
@@ -4370,19 +4408,19 @@
       </c>
       <c r="G13" s="27"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17">
       <c r="B14" s="26">
         <v>400</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
         <v>26666.666666666668</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
@@ -4390,19 +4428,19 @@
       </c>
       <c r="G14" s="27"/>
     </row>
-    <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:17" ht="15" thickBot="1">
       <c r="B15" s="28">
         <v>450</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D15" s="29">
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F15" s="29">
         <f t="shared" si="1"/>
@@ -4435,7 +4473,7 @@
       <selection pane="topRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
@@ -4451,51 +4489,51 @@
     <col min="17" max="17" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E1" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>158</v>
-      </c>
       <c r="J1" s="34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>19</v>
@@ -4504,15 +4542,15 @@
         <v>20</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" s="16">
         <v>0</v>
@@ -4563,15 +4601,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18">
       <c r="A3" s="33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B3" s="16">
         <v>0</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" s="16">
         <v>0</v>
@@ -4619,9 +4657,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18">
       <c r="A4" s="33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B4" s="16">
         <v>0</v>
@@ -4630,7 +4668,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>22</v>
@@ -4675,9 +4713,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18">
       <c r="A5" s="34" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -4707,10 +4745,10 @@
         <v>0</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
@@ -4731,9 +4769,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18">
       <c r="A6" s="34" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -4763,10 +4801,10 @@
         <v>0</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -4787,9 +4825,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18">
       <c r="A7" s="34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -4819,10 +4857,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M7" s="3">
         <v>0</v>
@@ -4843,9 +4881,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18">
       <c r="A8" s="34" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -4875,10 +4913,10 @@
         <v>0</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
@@ -4899,9 +4937,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18">
       <c r="A9" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -4931,10 +4969,10 @@
         <v>0</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L9" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
@@ -4955,9 +4993,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18">
       <c r="A10" s="34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -4987,10 +5025,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
@@ -5011,9 +5049,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18">
       <c r="A11" s="35" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -5067,9 +5105,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18">
       <c r="A12" s="35" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -5123,9 +5161,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18">
       <c r="A13" s="35" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -5179,9 +5217,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18">
       <c r="A14" s="35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -5235,9 +5273,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18">
       <c r="A15" s="35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -5291,7 +5329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18">
       <c r="A16" s="36" t="s">
         <v>19</v>
       </c>
@@ -5347,7 +5385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18">
       <c r="A17" s="36" t="s">
         <v>20</v>
       </c>
@@ -5403,9 +5441,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18">
       <c r="A18" s="37" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -5481,12 +5519,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I18" sqref="I18"/>
+      <selection pane="topRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17.26953125" customWidth="1"/>
@@ -5514,57 +5552,57 @@
     <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>29</v>
@@ -5573,48 +5611,48 @@
         <v>23</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V1" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B2" s="5">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F2" s="5">
         <v>0</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H2">
         <v>100</v>
       </c>
       <c r="I2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L2" s="5">
         <v>0</v>
@@ -5633,13 +5671,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -5648,42 +5686,42 @@
         <v>0</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F3" s="5">
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H3">
         <v>100</v>
       </c>
       <c r="I3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L3" s="5">
         <v>0</v>
@@ -5702,13 +5740,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -5717,42 +5755,42 @@
         <v>0</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F4" s="5">
         <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H4">
         <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L4" s="5">
         <v>0</v>
@@ -5771,13 +5809,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -5786,42 +5824,42 @@
         <v>0</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="22" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F5" s="5">
         <v>0</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H5">
         <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L5" s="5">
         <v>0</v>
@@ -5840,13 +5878,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -5855,42 +5893,42 @@
         <v>0</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F6" s="5">
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H6">
         <v>100</v>
       </c>
       <c r="I6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L6" s="5">
         <v>0</v>
@@ -5909,13 +5947,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -5924,67 +5962,67 @@
         <v>0</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F7" s="31">
         <v>0</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H7">
         <v>100</v>
       </c>
       <c r="I7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L7" s="31" t="s">
         <v>46</v>
       </c>
       <c r="M7" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="N7" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="O7" s="31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>54</v>
+        <v>231</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -5993,42 +6031,42 @@
         <v>0</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B8" s="5">
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="I8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L8" s="5">
         <v>0</v>
@@ -6040,19 +6078,19 @@
         <v>0</v>
       </c>
       <c r="O8" s="31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P8">
         <v>0.05</v>
       </c>
       <c r="Q8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R8" s="5">
         <v>0</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -6064,21 +6102,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23">
       <c r="A9" s="21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9" s="5">
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F9" s="5">
         <v>0</v>
@@ -6090,13 +6128,13 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="L9" s="5">
         <v>0</v>
@@ -6115,13 +6153,13 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="Q9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R9" s="5">
         <v>0</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="T9">
         <v>0</v>
@@ -6133,21 +6171,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23">
       <c r="A10" s="21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B10" s="5">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F10" s="5">
         <v>0</v>
@@ -6159,37 +6197,37 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="L10" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M10" s="5">
         <v>0</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="P10">
-        <v>0.1</v>
+        <v>218</v>
+      </c>
+      <c r="P10" s="48">
+        <v>0.08</v>
       </c>
       <c r="Q10" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R10" s="5">
         <v>0</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -6198,24 +6236,24 @@
         <v>0</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B11" s="5">
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
@@ -6227,63 +6265,63 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="L11" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="O11" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="P11">
+        <v>0.08</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>223</v>
+      </c>
+      <c r="R11" s="5">
+        <v>0</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="V11" t="s">
+        <v>98</v>
+      </c>
+      <c r="W11" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="M11" s="5">
-        <v>0</v>
-      </c>
-      <c r="N11" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="O11" s="31" t="s">
-        <v>221</v>
-      </c>
-      <c r="P11">
-        <v>0.1</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>226</v>
-      </c>
-      <c r="R11" s="5">
-        <v>0</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="V11" t="s">
-        <v>101</v>
-      </c>
-      <c r="W11" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="21" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B12" s="5">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F12" s="5">
         <v>0</v>
@@ -6295,37 +6333,37 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M12" s="5">
         <v>0</v>
       </c>
       <c r="N12" s="31" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O12" s="31" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P12">
         <v>0.08</v>
       </c>
       <c r="Q12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R12" s="5">
         <v>0</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="T12">
         <v>0</v>
@@ -6334,7 +6372,7 @@
         <v>0</v>
       </c>
       <c r="W12" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -6353,7 +6391,7 @@
       <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17.36328125" customWidth="1"/>
     <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
@@ -6367,65 +6405,65 @@
     <col min="12" max="12" width="30.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B2">
         <v>1E-3</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>2.2000000000000002</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F2" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -6437,33 +6475,33 @@
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B3">
         <v>1E-3</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D3">
         <v>2.2000000000000002</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F3" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -6475,33 +6513,33 @@
         <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B4">
         <v>1E-3</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>2.2000000000000002</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F4" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H4">
         <v>1000</v>
@@ -6513,33 +6551,33 @@
         <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="22" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B5">
         <v>1E-3</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5">
         <v>2.2000000000000002</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F5" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -6551,33 +6589,33 @@
         <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B6">
         <v>1E-3</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D6">
         <v>2.2000000000000002</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F6" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H6">
         <v>1000</v>
@@ -6589,33 +6627,33 @@
         <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>1E-3</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D7">
         <v>2.2000000000000002</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F7" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H7">
         <v>1000</v>
@@ -6627,33 +6665,33 @@
         <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B8">
         <v>0.05</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D8">
         <v>2.2000000000000002</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F8" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H8">
         <v>1000</v>
@@ -6665,33 +6703,33 @@
         <v>10</v>
       </c>
       <c r="K8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D9">
         <v>2.2000000000000002</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F9" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H9">
         <v>1000</v>
@@ -6703,33 +6741,33 @@
         <v>10</v>
       </c>
       <c r="K9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>2.2000000000000002</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F10" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H10">
         <v>1000</v>
@@ -6741,33 +6779,33 @@
         <v>10</v>
       </c>
       <c r="K10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>2.2000000000000002</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F11" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H11">
         <v>1000</v>
@@ -6779,33 +6817,33 @@
         <v>10</v>
       </c>
       <c r="K11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="21" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D12">
         <v>2.2000000000000002</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F12" s="46">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H12">
         <v>1000</v>
@@ -6817,10 +6855,10 @@
         <v>10</v>
       </c>
       <c r="K12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -6834,12 +6872,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B92B1C5-379D-4587-B23B-6C3AF487A07D}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
@@ -6855,51 +6893,51 @@
     <col min="17" max="17" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E1" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>158</v>
-      </c>
       <c r="J1" s="34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>19</v>
@@ -6908,15 +6946,15 @@
         <v>20</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C2" s="16">
         <v>0</v>
@@ -6967,15 +7005,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18">
       <c r="A3" s="33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B3" s="16">
         <v>0</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D3" s="16">
         <v>0</v>
@@ -7023,9 +7061,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18">
       <c r="A4" s="33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B4" s="16">
         <v>0</v>
@@ -7034,7 +7072,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -7079,9 +7117,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18">
       <c r="A5" s="34" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -7093,7 +7131,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -7135,9 +7173,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18">
       <c r="A6" s="34" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -7152,7 +7190,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -7191,9 +7229,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18">
       <c r="A7" s="34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -7211,7 +7249,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
@@ -7247,9 +7285,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18">
       <c r="A8" s="34" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -7270,7 +7308,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -7303,9 +7341,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18">
       <c r="A9" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -7329,7 +7367,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
@@ -7359,9 +7397,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18">
       <c r="A10" s="34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -7388,7 +7426,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>24</v>
@@ -7415,9 +7453,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18">
       <c r="A11" s="35" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -7447,7 +7485,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L11" s="1">
         <v>0</v>
@@ -7471,9 +7509,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18">
       <c r="A12" s="35" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -7506,7 +7544,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="M12" s="1">
         <v>0</v>
@@ -7527,9 +7565,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18">
       <c r="A13" s="35" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -7583,9 +7621,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18">
       <c r="A14" s="35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -7639,9 +7677,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18">
       <c r="A15" s="35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -7695,7 +7733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18">
       <c r="A16" s="36" t="s">
         <v>19</v>
       </c>
@@ -7751,7 +7789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18">
       <c r="A17" s="36" t="s">
         <v>20</v>
       </c>
@@ -7807,9 +7845,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18">
       <c r="A18" s="37" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -7883,14 +7921,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8D8FB7-0FD2-42C3-9D82-0A6D9AE32488}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="41.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.6328125" bestFit="1" customWidth="1"/>
@@ -7898,11 +7936,11 @@
     <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -7916,7 +7954,7 @@
         <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>35</v>
@@ -7928,148 +7966,148 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="B5" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="C5" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="H5" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G6" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="32" t="s">
-        <v>54</v>
+        <v>231</v>
       </c>
       <c r="B7" s="13">
         <v>0</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>14</v>
@@ -8077,16 +8115,16 @@
       <c r="F7" s="14">
         <v>0</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>48</v>
+      <c r="G7" s="47" t="s">
+        <v>232</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="42" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -8095,6 +8133,9 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="G9" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8110,66 +8151,66 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M1" t="s">
+        <v>190</v>
+      </c>
+      <c r="N1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="F1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" t="s">
-        <v>189</v>
-      </c>
-      <c r="J1" t="s">
-        <v>190</v>
-      </c>
-      <c r="K1" t="s">
-        <v>191</v>
-      </c>
-      <c r="L1" t="s">
-        <v>192</v>
-      </c>
-      <c r="M1" t="s">
-        <v>193</v>
-      </c>
-      <c r="N1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>215</v>
-      </c>
       <c r="C2" s="43" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D2" s="44">
         <v>0.95</v>
@@ -8196,10 +8237,10 @@
         <v>0.5</v>
       </c>
       <c r="K2" s="45" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L2" s="45" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="M2" s="45">
         <v>100</v>
@@ -8208,15 +8249,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14">
       <c r="A3" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>216</v>
-      </c>
       <c r="C3" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D3" s="14">
         <v>0.95</v>
@@ -8243,10 +8284,10 @@
         <v>0.5</v>
       </c>
       <c r="K3" s="45" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L3" s="45" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="M3" s="45">
         <v>100</v>
@@ -8255,15 +8296,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14">
       <c r="A4" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>217</v>
-      </c>
       <c r="C4" s="13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D4" s="14">
         <v>0.95</v>
@@ -8290,10 +8331,10 @@
         <v>0.5</v>
       </c>
       <c r="K4" s="45" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L4" s="45" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="M4" s="45">
         <v>100</v>
@@ -8315,12 +8356,12 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="11" t="s">
         <v>38</v>
       </c>
@@ -8328,7 +8369,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -8336,7 +8377,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -8344,7 +8385,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -8352,7 +8393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -8360,7 +8401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -8368,7 +8409,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -8376,7 +8417,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -8384,52 +8425,52 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
         <v>129</v>
       </c>
-      <c r="B10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s">
         <v>130</v>
-      </c>
-      <c r="B12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -8445,141 +8486,141 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>184</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
         <v>195</v>
       </c>
-      <c r="C2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>185</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
         <v>196</v>
       </c>
-      <c r="C3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" t="s">
         <v>197</v>
       </c>
-      <c r="C4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>188</v>
       </c>
-      <c r="B6" t="s">
-        <v>201</v>
-      </c>
-      <c r="C6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>189</v>
       </c>
-      <c r="B7" t="s">
-        <v>199</v>
-      </c>
-      <c r="C7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>190</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>200</v>
       </c>
-      <c r="C8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="C11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>191</v>
       </c>
-      <c r="B9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C9" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>192</v>
-      </c>
-      <c r="B10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>203</v>
       </c>
-      <c r="C11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>194</v>
-      </c>
-      <c r="B12" t="s">
-        <v>206</v>
-      </c>
       <c r="C12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -8595,7 +8636,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
@@ -8606,47 +8647,47 @@
     <col min="9" max="11" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="K3" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
@@ -8654,31 +8695,31 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" t="s">
         <v>104</v>
       </c>
-      <c r="G4" t="s">
-        <v>107</v>
-      </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
@@ -8686,31 +8727,31 @@
         <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" t="s">
         <v>104</v>
       </c>
-      <c r="G5" t="s">
-        <v>107</v>
-      </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
@@ -8718,31 +8759,31 @@
         <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" t="s">
         <v>104</v>
       </c>
-      <c r="G6" t="s">
-        <v>107</v>
-      </c>
       <c r="H6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
@@ -8750,31 +8791,31 @@
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" t="s">
         <v>104</v>
       </c>
-      <c r="G7" t="s">
-        <v>107</v>
-      </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="22" t="s">
         <v>26</v>
       </c>
@@ -8782,205 +8823,205 @@
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="39" t="s">
         <v>227</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="38">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" t="s">
         <v>104</v>
       </c>
-      <c r="G8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H8" t="s">
-        <v>107</v>
-      </c>
-      <c r="I8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J8" t="s">
-        <v>107</v>
-      </c>
-      <c r="K8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="D9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="H11" t="s">
         <v>104</v>
       </c>
-      <c r="G9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H9" t="s">
-        <v>107</v>
-      </c>
-      <c r="I9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J9" t="s">
-        <v>107</v>
-      </c>
-      <c r="K9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="I11" t="s">
+        <v>104</v>
+      </c>
+      <c r="J11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="E12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" t="s">
         <v>104</v>
       </c>
-      <c r="G10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" t="s">
-        <v>107</v>
-      </c>
-      <c r="I10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J10" t="s">
-        <v>107</v>
-      </c>
-      <c r="K10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="38">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="H12" t="s">
         <v>104</v>
       </c>
-      <c r="G11" t="s">
-        <v>107</v>
-      </c>
-      <c r="H11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I11" t="s">
-        <v>107</v>
-      </c>
-      <c r="J11" t="s">
-        <v>107</v>
-      </c>
-      <c r="K11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="I12" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" t="s">
         <v>104</v>
       </c>
-      <c r="G12" t="s">
-        <v>107</v>
-      </c>
-      <c r="H12" t="s">
-        <v>107</v>
-      </c>
-      <c r="I12" t="s">
-        <v>107</v>
-      </c>
-      <c r="J12" t="s">
-        <v>107</v>
-      </c>
-      <c r="K12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="H13" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" t="s">
+        <v>104</v>
+      </c>
+      <c r="K13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" t="s">
         <v>104</v>
       </c>
-      <c r="G13" t="s">
-        <v>107</v>
-      </c>
-      <c r="H13" t="s">
-        <v>107</v>
-      </c>
-      <c r="I13" t="s">
-        <v>107</v>
-      </c>
-      <c r="J13" t="s">
-        <v>107</v>
-      </c>
-      <c r="K13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" t="s">
-        <v>229</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
         <v>104</v>
       </c>
-      <c r="G14" t="s">
-        <v>107</v>
-      </c>
-      <c r="H14" t="s">
-        <v>107</v>
-      </c>
       <c r="I14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes to surrogate models (sbml + open fermentation)
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC772A2E-0922-44B8-A33E-1A0C7A1F3F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B45845-4760-4F16-A308-26ED55FC3376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="connection_matrix_old" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3845,8 +3846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE4236-3006-4E07-A9E2-DEE610CD0DBE}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3898,10 +3899,10 @@
         <v>53</v>
       </c>
       <c r="C2">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="D2">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="E2">
         <v>0.56999999999999995</v>
@@ -3924,10 +3925,10 @@
         <v>54</v>
       </c>
       <c r="C3">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="D3">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="E3">
         <v>0.39</v>
@@ -3950,10 +3951,10 @@
         <v>105</v>
       </c>
       <c r="C4">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="D4">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="E4">
         <v>0.35</v>
@@ -3985,7 +3986,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>17</v>
@@ -4011,7 +4012,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>16</v>
@@ -5519,8 +5520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
@@ -6388,7 +6389,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
add water equations to superstructure DONE
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B45845-4760-4F16-A308-26ED55FC3376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183479A7-FC9D-4301-BC69-0A4BF4EA8F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
@@ -26,7 +26,6 @@
     <sheet name="connection_matrix_old" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="234">
   <si>
     <t>components</t>
   </si>
@@ -458,9 +457,6 @@
     <t>Ex_S_cpd00027_ext, Ex_S_cpd00082_ext, Ex_S_cpd00100_ext</t>
   </si>
   <si>
-    <t>Propionate, Acetate, Biomass</t>
-  </si>
-  <si>
     <t>Ex_S_cpd00141_ext, Ex_S_cpd00029_ext, Ex_S_biomass_ext</t>
   </si>
   <si>
@@ -468,9 +464,6 @@
   </si>
   <si>
     <t>bm</t>
-  </si>
-  <si>
-    <t>prop, ace, bm</t>
   </si>
   <si>
     <t>[0.95, 0.95, 0.95, 0.05] ; [0.05, 0.05, 0.05, 0.95]</t>
@@ -754,6 +747,12 @@
   </si>
   <si>
     <t>open_fermentation_polynomial_case_study.json</t>
+  </si>
+  <si>
+    <t>Propionate, Acetate, Biomass, water</t>
+  </si>
+  <si>
+    <t>prop, ace, bm, water</t>
   </si>
   <si>
     <r>
@@ -776,11 +775,11 @@
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> CV_Propionate, CV_Biomass</t>
+      <t xml:space="preserve"> CV_Propionate, CV_Biomass, water</t>
     </r>
   </si>
   <si>
-    <t>ace, prop, bm</t>
+    <t>ace, prop, bm, water</t>
   </si>
 </sst>
 </file>
@@ -3847,7 +3846,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3986,7 +3985,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>17</v>
@@ -4012,7 +4011,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>1.26</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>16</v>
@@ -4091,13 +4090,13 @@
         <v>105</v>
       </c>
       <c r="N4" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O4" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q4" s="40" t="s">
         <v>17</v>
@@ -4213,7 +4212,7 @@
         <v>66.666666666666671</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K8" s="5">
         <v>0</v>
@@ -4225,16 +4224,16 @@
         <v>0</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O8" s="5">
         <v>0</v>
       </c>
       <c r="P8" s="41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Q8" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="2:17">
@@ -4257,7 +4256,7 @@
         <v>66.666666666666671</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K9" s="5">
         <v>0</v>
@@ -4272,13 +4271,13 @@
         <v>0</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="P9" s="41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Q9" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="2:17">
@@ -4301,7 +4300,7 @@
       </c>
       <c r="G10" s="27"/>
       <c r="J10" s="40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K10" s="5">
         <v>0</v>
@@ -4504,19 +4503,19 @@
         <v>105</v>
       </c>
       <c r="E1" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>153</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>155</v>
       </c>
       <c r="J1" s="34" t="s">
         <v>47</v>
@@ -4528,13 +4527,13 @@
         <v>65</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>19</v>
@@ -4716,7 +4715,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -4772,7 +4771,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -4828,7 +4827,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -4884,7 +4883,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -4940,7 +4939,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -5164,7 +5163,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -5220,7 +5219,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -5276,7 +5275,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -5521,8 +5520,8 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R7" sqref="R7"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5567,7 +5566,7 @@
         <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>119</v>
@@ -5585,22 +5584,22 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>71</v>
@@ -5623,16 +5622,16 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2" s="5">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>89</v>
@@ -5640,17 +5639,17 @@
       <c r="F2" s="5">
         <v>0</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>128</v>
+      <c r="G2" s="5">
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I2" t="s">
         <v>111</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>89</v>
@@ -5672,13 +5671,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>112</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -5692,13 +5691,13 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>120</v>
@@ -5709,17 +5708,17 @@
       <c r="F3" s="5">
         <v>0</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>128</v>
+      <c r="G3" s="5">
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I3" t="s">
         <v>111</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>89</v>
@@ -5741,13 +5740,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>113</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -5761,16 +5760,16 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>89</v>
@@ -5778,17 +5777,17 @@
       <c r="F4" s="5">
         <v>0</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>128</v>
+      <c r="G4" s="5">
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I4" t="s">
         <v>111</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>89</v>
@@ -5810,13 +5809,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>114</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -5830,16 +5829,16 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>89</v>
@@ -5847,17 +5846,17 @@
       <c r="F5" s="5">
         <v>0</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>128</v>
+      <c r="G5" s="5">
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I5" t="s">
         <v>111</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>89</v>
@@ -5879,13 +5878,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>115</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -5899,16 +5898,16 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>89</v>
@@ -5916,17 +5915,17 @@
       <c r="F6" s="5">
         <v>0</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>128</v>
+      <c r="G6" s="5">
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I6" t="s">
         <v>111</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>89</v>
@@ -5948,13 +5947,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>116</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -5974,7 +5973,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>14</v>
@@ -5985,17 +5984,17 @@
       <c r="F7" s="31">
         <v>0</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>128</v>
+      <c r="G7" s="5">
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I7" t="s">
         <v>111</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>89</v>
@@ -6010,20 +6009,20 @@
         <v>121</v>
       </c>
       <c r="O7" s="31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -6043,7 +6042,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>123</v>
@@ -6079,19 +6078,19 @@
         <v>0</v>
       </c>
       <c r="O8" s="31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P8">
         <v>0.05</v>
       </c>
       <c r="Q8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R8" s="5">
         <v>0</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -6111,7 +6110,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>90</v>
@@ -6154,13 +6153,13 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="Q9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R9" s="5">
         <v>0</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="T9">
         <v>0</v>
@@ -6174,13 +6173,13 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B10" s="5">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>122</v>
@@ -6207,28 +6206,28 @@
         <v>89</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M10" s="5">
         <v>0</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="P10" s="48">
         <v>0.08</v>
       </c>
       <c r="Q10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R10" s="5">
         <v>0</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -6242,13 +6241,13 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B11" s="5">
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>123</v>
@@ -6275,28 +6274,28 @@
         <v>89</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M11" s="5">
         <v>0</v>
       </c>
       <c r="N11" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="O11" s="31" t="s">
         <v>216</v>
-      </c>
-      <c r="O11" s="31" t="s">
-        <v>218</v>
       </c>
       <c r="P11">
         <v>0.08</v>
       </c>
       <c r="Q11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R11" s="5">
         <v>0</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="T11">
         <v>0</v>
@@ -6310,13 +6309,13 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B12" s="5">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>124</v>
@@ -6343,28 +6342,28 @@
         <v>89</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M12" s="5">
         <v>0</v>
       </c>
       <c r="N12" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="O12" s="31" t="s">
         <v>216</v>
-      </c>
-      <c r="O12" s="31" t="s">
-        <v>218</v>
       </c>
       <c r="P12">
         <v>0.08</v>
       </c>
       <c r="Q12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R12" s="5">
         <v>0</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="T12">
         <v>0</v>
@@ -6389,7 +6388,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6446,7 +6445,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2">
         <v>1E-3</v>
@@ -6484,7 +6483,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3">
         <v>1E-3</v>
@@ -6522,7 +6521,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B4">
         <v>1E-3</v>
@@ -6560,7 +6559,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B5">
         <v>1E-3</v>
@@ -6598,7 +6597,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B6">
         <v>1E-3</v>
@@ -6750,7 +6749,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -6788,7 +6787,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6826,7 +6825,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -6908,19 +6907,19 @@
         <v>105</v>
       </c>
       <c r="E1" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>153</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>155</v>
       </c>
       <c r="J1" s="34" t="s">
         <v>47</v>
@@ -6932,13 +6931,13 @@
         <v>65</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>19</v>
@@ -6955,7 +6954,7 @@
         <v>53</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C2" s="16">
         <v>0</v>
@@ -7014,7 +7013,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D3" s="16">
         <v>0</v>
@@ -7073,7 +7072,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -7120,7 +7119,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -7132,7 +7131,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -7176,7 +7175,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -7191,7 +7190,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -7232,7 +7231,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -7250,7 +7249,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
@@ -7288,7 +7287,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -7309,7 +7308,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -7344,7 +7343,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -7368,7 +7367,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
@@ -7427,7 +7426,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>24</v>
@@ -7486,7 +7485,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L11" s="1">
         <v>0</v>
@@ -7545,7 +7544,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M12" s="1">
         <v>0</v>
@@ -7568,7 +7567,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -7624,7 +7623,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -7680,7 +7679,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -7925,8 +7924,8 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G16" sqref="G16"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -7937,8 +7936,8 @@
     <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7984,13 +7983,13 @@
         <v>135</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -8010,13 +8009,13 @@
         <v>60</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -8036,13 +8035,13 @@
         <v>135</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -8062,13 +8061,13 @@
         <v>135</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -8088,18 +8087,18 @@
         <v>135</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="32" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B7" s="13">
         <v>0</v>
@@ -8125,7 +8124,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="42" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -8164,51 +8163,51 @@
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>184</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>185</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>186</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>187</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>188</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>189</v>
-      </c>
-      <c r="M1" t="s">
-        <v>190</v>
-      </c>
-      <c r="N1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="42" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>85</v>
@@ -8238,10 +8237,10 @@
         <v>0.5</v>
       </c>
       <c r="K2" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="L2" s="45" t="s">
         <v>204</v>
-      </c>
-      <c r="L2" s="45" t="s">
-        <v>206</v>
       </c>
       <c r="M2" s="45">
         <v>100</v>
@@ -8252,10 +8251,10 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="42" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>128</v>
@@ -8285,10 +8284,10 @@
         <v>0.5</v>
       </c>
       <c r="K3" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="L3" s="45" t="s">
         <v>204</v>
-      </c>
-      <c r="L3" s="45" t="s">
-        <v>206</v>
       </c>
       <c r="M3" s="45">
         <v>100</v>
@@ -8299,13 +8298,13 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="42" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D4" s="14">
         <v>0.95</v>
@@ -8332,10 +8331,10 @@
         <v>0.5</v>
       </c>
       <c r="K4" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="L4" s="45" t="s">
         <v>204</v>
-      </c>
-      <c r="L4" s="45" t="s">
-        <v>206</v>
       </c>
       <c r="M4" s="45">
         <v>100</v>
@@ -8468,7 +8467,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
         <v>130</v>
@@ -8494,10 +8493,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C1" t="s">
         <v>71</v>
@@ -8505,123 +8504,123 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -8696,10 +8695,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E4" t="s">
         <v>101</v>
@@ -8728,10 +8727,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E5" t="s">
         <v>101</v>
@@ -8760,10 +8759,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E6" t="s">
         <v>101</v>
@@ -8792,10 +8791,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E7" t="s">
         <v>101</v>
@@ -8824,10 +8823,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E8" t="s">
         <v>101</v>
@@ -8856,10 +8855,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E9" t="s">
         <v>101</v>
@@ -8885,10 +8884,10 @@
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E10" t="s">
         <v>101</v>
@@ -8917,7 +8916,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E11" t="s">
         <v>101</v>
@@ -8943,10 +8942,10 @@
         <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E12" t="s">
         <v>101</v>
@@ -8972,10 +8971,10 @@
         <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E13" t="s">
         <v>101</v>
@@ -9001,10 +9000,10 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E14" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
experimenting on adding compartments to models
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183479A7-FC9D-4301-BC69-0A4BF4EA8F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55463684-73A1-4E31-A540-AAADDE38160E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" firstSheet="1" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="238">
   <si>
     <t>components</t>
   </si>
@@ -349,16 +349,10 @@
     <t>cost_waste</t>
   </si>
   <si>
-    <t>lala et al (2022)</t>
-  </si>
-  <si>
     <t>REFERENCES process parameters</t>
   </si>
   <si>
     <t>REFERENCES economic parameters</t>
-  </si>
-  <si>
-    <t>smthing et al (2023)</t>
   </si>
   <si>
     <t>carbon_input3</t>
@@ -731,16 +725,10 @@
     <t>McCubbin et al</t>
   </si>
   <si>
-    <t>Patent mateo</t>
-  </si>
-  <si>
     <t>TOFIND</t>
   </si>
   <si>
     <t>Koyuncu et al (2000)</t>
-  </si>
-  <si>
-    <t>processing principles book</t>
   </si>
   <si>
     <t>Reguiera et al (2018)</t>
@@ -781,12 +769,36 @@
   <si>
     <t>ace, prop, bm, water</t>
   </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s13068-019-1433-8</t>
+  </si>
+  <si>
+    <t>processing principles book (short cut)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seperation efficientcy </t>
+  </si>
+  <si>
+    <t>TOFIND (see DWA?)</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s13068-019-1433-7</t>
+  </si>
+  <si>
+    <t>mu_ut (added chemicals)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -834,6 +846,19 @@
       <color rgb="FF008000"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -910,7 +935,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1070,11 +1095,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1164,6 +1228,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2298,16 +2371,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>429472</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>90805</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>84030</xdr:rowOff>
+      <xdr:rowOff>105197</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>309456</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>140123</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>138007</xdr:rowOff>
+      <xdr:rowOff>159174</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2322,8 +2395,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11446722" y="3398730"/>
-          <a:ext cx="2889884" cy="3736977"/>
+          <a:off x="11908861" y="3421308"/>
+          <a:ext cx="2885651" cy="3722866"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2521,50 +2594,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>486953</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>98326</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>189374</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>3628</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{629B3289-EFEB-4A7A-B778-1BC14A780257}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5712096" y="3445683"/>
-          <a:ext cx="5489992" cy="2322838"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
@@ -2708,6 +2737,50 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>787084</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>74082</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>202534</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>163992</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94254927-E313-BA75-FA91-003151D0909A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6015251" y="3603624"/>
+          <a:ext cx="5992991" cy="2497618"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3194,13 +3267,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>48260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
@@ -3845,8 +3918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE4236-3006-4E07-A9E2-DEE610CD0DBE}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D22" sqref="D21:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3947,7 +4020,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4">
         <v>500</v>
@@ -3962,7 +4035,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -4052,7 +4125,7 @@
   <sheetData>
     <row r="2" spans="2:17" ht="15" thickBot="1">
       <c r="B2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="2:17">
@@ -4087,16 +4160,16 @@
         <v>54</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N4" s="34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O4" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Q4" s="40" t="s">
         <v>17</v>
@@ -4168,16 +4241,16 @@
       <c r="B7" s="26"/>
       <c r="G7" s="27"/>
       <c r="J7" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0</v>
+      </c>
+      <c r="M7" s="16" t="s">
         <v>105</v>
-      </c>
-      <c r="K7" s="16">
-        <v>0</v>
-      </c>
-      <c r="L7" s="16">
-        <v>0</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>107</v>
       </c>
       <c r="N7" s="10">
         <v>1</v>
@@ -4212,7 +4285,7 @@
         <v>66.666666666666671</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K8" s="5">
         <v>0</v>
@@ -4224,16 +4297,16 @@
         <v>0</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O8" s="5">
         <v>0</v>
       </c>
       <c r="P8" s="41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q8" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="2:17">
@@ -4256,7 +4329,7 @@
         <v>66.666666666666671</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K9" s="5">
         <v>0</v>
@@ -4271,13 +4344,13 @@
         <v>0</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P9" s="41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q9" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="2:17">
@@ -4300,7 +4373,7 @@
       </c>
       <c r="G10" s="27"/>
       <c r="J10" s="40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K10" s="5">
         <v>0</v>
@@ -4500,22 +4573,22 @@
         <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E1" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>151</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>153</v>
       </c>
       <c r="J1" s="34" t="s">
         <v>47</v>
@@ -4527,13 +4600,13 @@
         <v>65</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>19</v>
@@ -4542,7 +4615,7 @@
         <v>20</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -4659,16 +4732,16 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>105</v>
-      </c>
-      <c r="B4" s="16">
-        <v>0</v>
-      </c>
-      <c r="C4" s="16">
-        <v>0</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>107</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>22</v>
@@ -4715,7 +4788,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -4745,10 +4818,10 @@
         <v>0</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
@@ -4771,7 +4844,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -4801,10 +4874,10 @@
         <v>0</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -4827,7 +4900,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -4857,10 +4930,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M7" s="3">
         <v>0</v>
@@ -4883,7 +4956,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -4913,10 +4986,10 @@
         <v>0</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
@@ -4939,7 +5012,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -4969,10 +5042,10 @@
         <v>0</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L9" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
@@ -5025,10 +5098,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
@@ -5163,7 +5236,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="35" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -5219,7 +5292,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="35" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -5275,7 +5348,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -5443,7 +5516,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="37" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -5521,7 +5594,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I18" sqref="I18"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5557,19 +5630,19 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>79</v>
@@ -5584,22 +5657,22 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>71</v>
@@ -5622,16 +5695,16 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B2" s="5">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>89</v>
@@ -5646,10 +5719,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>89</v>
@@ -5671,13 +5744,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -5691,16 +5764,16 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>89</v>
@@ -5715,10 +5788,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>89</v>
@@ -5740,13 +5813,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -5760,16 +5833,16 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>89</v>
@@ -5784,10 +5857,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>89</v>
@@ -5809,13 +5882,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -5829,16 +5902,16 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>89</v>
@@ -5853,10 +5926,10 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>89</v>
@@ -5878,13 +5951,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -5898,16 +5971,16 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>89</v>
@@ -5922,10 +5995,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>89</v>
@@ -5947,13 +6020,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -5973,7 +6046,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>14</v>
@@ -5991,10 +6064,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>89</v>
@@ -6003,26 +6076,26 @@
         <v>46</v>
       </c>
       <c r="M7" s="31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N7" s="31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O7" s="31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="Q7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -6042,10 +6115,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>89</v>
@@ -6057,10 +6130,10 @@
         <v>85</v>
       </c>
       <c r="H8">
-        <v>5.7000000000000002E-2</v>
+        <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>91</v>
@@ -6078,19 +6151,19 @@
         <v>0</v>
       </c>
       <c r="O8" s="31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P8">
         <v>0.05</v>
       </c>
       <c r="Q8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R8" s="5">
         <v>0</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -6110,7 +6183,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>90</v>
@@ -6153,13 +6226,13 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="Q9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R9" s="5">
         <v>0</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T9">
         <v>0</v>
@@ -6173,16 +6246,16 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B10" s="5">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>89</v>
@@ -6206,28 +6279,28 @@
         <v>89</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M10" s="5">
         <v>0</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P10" s="48">
         <v>0.08</v>
       </c>
       <c r="Q10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R10" s="5">
         <v>0</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -6241,16 +6314,16 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B11" s="5">
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>89</v>
@@ -6274,28 +6347,28 @@
         <v>89</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M11" s="5">
         <v>0</v>
       </c>
       <c r="N11" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="O11" s="31" t="s">
         <v>214</v>
-      </c>
-      <c r="O11" s="31" t="s">
-        <v>216</v>
       </c>
       <c r="P11">
         <v>0.08</v>
       </c>
       <c r="Q11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R11" s="5">
         <v>0</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="T11">
         <v>0</v>
@@ -6309,16 +6382,16 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B12" s="5">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>89</v>
@@ -6342,28 +6415,28 @@
         <v>89</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M12" s="5">
         <v>0</v>
       </c>
       <c r="N12" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="O12" s="31" t="s">
         <v>214</v>
-      </c>
-      <c r="O12" s="31" t="s">
-        <v>216</v>
       </c>
       <c r="P12">
         <v>0.08</v>
       </c>
       <c r="Q12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R12" s="5">
         <v>0</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="T12">
         <v>0</v>
@@ -6445,7 +6518,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B2">
         <v>1E-3</v>
@@ -6483,7 +6556,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3">
         <v>1E-3</v>
@@ -6521,7 +6594,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4">
         <v>1E-3</v>
@@ -6559,7 +6632,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5">
         <v>1E-3</v>
@@ -6597,7 +6670,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B6">
         <v>1E-3</v>
@@ -6749,7 +6822,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -6787,7 +6860,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6825,7 +6898,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -6872,9 +6945,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B92B1C5-379D-4587-B23B-6C3AF487A07D}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -6904,22 +6977,22 @@
         <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E1" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>151</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>153</v>
       </c>
       <c r="J1" s="34" t="s">
         <v>47</v>
@@ -6931,13 +7004,13 @@
         <v>65</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>19</v>
@@ -6946,7 +7019,7 @@
         <v>20</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -6954,7 +7027,7 @@
         <v>53</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C2" s="16">
         <v>0</v>
@@ -7013,7 +7086,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D3" s="16">
         <v>0</v>
@@ -7063,7 +7136,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="16">
         <v>0</v>
@@ -7072,7 +7145,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -7119,7 +7192,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -7131,7 +7204,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -7175,7 +7248,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -7190,7 +7263,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -7231,7 +7304,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -7249,7 +7322,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
@@ -7287,7 +7360,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -7308,7 +7381,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -7343,7 +7416,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -7367,7 +7440,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
@@ -7426,7 +7499,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>24</v>
@@ -7485,7 +7558,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L11" s="1">
         <v>0</v>
@@ -7509,7 +7582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" ht="15" thickBot="1">
       <c r="A12" s="35" t="s">
         <v>65</v>
       </c>
@@ -7540,11 +7613,11 @@
       <c r="J12" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="52">
         <v>0</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="M12" s="1">
         <v>0</v>
@@ -7565,9 +7638,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" ht="15" thickBot="1">
       <c r="A13" s="35" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -7593,37 +7666,37 @@
       <c r="I13" s="1">
         <v>0</v>
       </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="1">
+      <c r="J13" s="51">
+        <v>0</v>
+      </c>
+      <c r="K13" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="32">
         <v>0</v>
       </c>
       <c r="M13" s="1">
         <v>0</v>
       </c>
-      <c r="N13" s="7" t="s">
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
       <c r="P13" s="1">
         <v>0</v>
       </c>
       <c r="Q13" s="1">
         <v>0</v>
       </c>
-      <c r="R13" s="7" t="s">
-        <v>25</v>
+      <c r="R13" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="35" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -7652,7 +7725,7 @@
       <c r="J14" s="1">
         <v>0</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="50">
         <v>0</v>
       </c>
       <c r="L14" s="1">
@@ -7679,7 +7752,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -7847,7 +7920,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="37" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -7968,33 +8041,33 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>137</v>
-      </c>
       <c r="G2" s="14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>55</v>
@@ -8009,96 +8082,96 @@
         <v>60</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>137</v>
-      </c>
       <c r="G4" s="14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>137</v>
-      </c>
       <c r="G5" s="14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>137</v>
-      </c>
       <c r="G6" s="14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="32" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B7" s="13">
         <v>0</v>
@@ -8116,15 +8189,15 @@
         <v>0</v>
       </c>
       <c r="G7" s="47" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="42" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -8163,51 +8236,51 @@
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>181</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>182</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>183</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>184</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>185</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>186</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>187</v>
-      </c>
-      <c r="M1" t="s">
-        <v>188</v>
-      </c>
-      <c r="N1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="42" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>85</v>
@@ -8237,10 +8310,10 @@
         <v>0.5</v>
       </c>
       <c r="K2" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="L2" s="45" t="s">
         <v>202</v>
-      </c>
-      <c r="L2" s="45" t="s">
-        <v>204</v>
       </c>
       <c r="M2" s="45">
         <v>100</v>
@@ -8251,13 +8324,13 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="42" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D3" s="14">
         <v>0.95</v>
@@ -8284,10 +8357,10 @@
         <v>0.5</v>
       </c>
       <c r="K3" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="L3" s="45" t="s">
         <v>202</v>
-      </c>
-      <c r="L3" s="45" t="s">
-        <v>204</v>
       </c>
       <c r="M3" s="45">
         <v>100</v>
@@ -8298,13 +8371,13 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="42" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D4" s="14">
         <v>0.95</v>
@@ -8331,10 +8404,10 @@
         <v>0.5</v>
       </c>
       <c r="K4" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="L4" s="45" t="s">
         <v>202</v>
-      </c>
-      <c r="L4" s="45" t="s">
-        <v>204</v>
       </c>
       <c r="M4" s="45">
         <v>100</v>
@@ -8435,26 +8508,26 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -8462,15 +8535,15 @@
         <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -8493,10 +8566,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C1" t="s">
         <v>71</v>
@@ -8504,123 +8577,123 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -8630,399 +8703,386 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE819A9C-4E64-4D0F-8F31-2F1BF4DCFD79}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.90625" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" customWidth="1"/>
-    <col min="9" max="11" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.90625" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" customWidth="1"/>
+    <col min="10" max="12" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>233</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" s="39" t="s">
+        <v>234</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="D4" t="s">
-        <v>223</v>
-      </c>
-      <c r="E4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" t="s">
-        <v>104</v>
-      </c>
-      <c r="I4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="H4" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" s="39" t="s">
+        <v>234</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="D5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I5" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" t="s">
-        <v>104</v>
-      </c>
-      <c r="K5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="H5" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J5" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" s="39" t="s">
+        <v>234</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="D6" t="s">
-        <v>223</v>
-      </c>
-      <c r="E6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" t="s">
-        <v>104</v>
-      </c>
-      <c r="I6" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" t="s">
-        <v>104</v>
-      </c>
-      <c r="K6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="H6" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" s="39" t="s">
+        <v>234</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F7" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="D7" t="s">
-        <v>223</v>
-      </c>
-      <c r="E7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J7" t="s">
-        <v>104</v>
-      </c>
-      <c r="K7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="H7" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" s="39" t="s">
+        <v>234</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F8" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="D8" t="s">
-        <v>223</v>
-      </c>
-      <c r="E8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G8" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" t="s">
-        <v>104</v>
-      </c>
-      <c r="I8" t="s">
-        <v>104</v>
-      </c>
-      <c r="J8" t="s">
-        <v>104</v>
-      </c>
-      <c r="K8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="H8" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" s="39" t="s">
+        <v>234</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F9" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="D9" t="s">
-        <v>228</v>
-      </c>
-      <c r="E9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G9" t="s">
-        <v>104</v>
-      </c>
-      <c r="H9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I9" t="s">
-        <v>104</v>
-      </c>
-      <c r="J9" t="s">
-        <v>104</v>
-      </c>
-      <c r="K9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="H9" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J9" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>224</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>225</v>
-      </c>
-      <c r="E10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H10" t="s">
-        <v>104</v>
-      </c>
-      <c r="I10" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" t="s">
-        <v>104</v>
-      </c>
-      <c r="K10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>235</v>
+      </c>
+      <c r="C10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="38">
-        <v>0</v>
+      <c r="B11" s="39" t="s">
+        <v>234</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="E11" t="s">
-        <v>101</v>
-      </c>
-      <c r="G11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" t="s">
-        <v>104</v>
-      </c>
-      <c r="J11" t="s">
-        <v>104</v>
-      </c>
-      <c r="K11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>230</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="21" t="s">
         <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E12" t="s">
-        <v>101</v>
-      </c>
-      <c r="G12" t="s">
-        <v>104</v>
-      </c>
-      <c r="H12" t="s">
-        <v>104</v>
-      </c>
-      <c r="I12" t="s">
-        <v>104</v>
-      </c>
-      <c r="J12" t="s">
-        <v>104</v>
-      </c>
-      <c r="K12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>230</v>
+      </c>
+      <c r="D12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="H12" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
-        <v>224</v>
+      <c r="B13" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" t="s">
-        <v>104</v>
-      </c>
-      <c r="H13" t="s">
-        <v>104</v>
-      </c>
-      <c r="I13" t="s">
-        <v>104</v>
-      </c>
-      <c r="J13" t="s">
-        <v>104</v>
-      </c>
-      <c r="K13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>230</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J13" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B14" t="s">
-        <v>224</v>
+      <c r="B14" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E14" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" t="s">
-        <v>104</v>
-      </c>
-      <c r="H14" t="s">
-        <v>104</v>
-      </c>
-      <c r="I14" t="s">
-        <v>104</v>
-      </c>
-      <c r="J14" t="s">
-        <v>104</v>
-      </c>
-      <c r="K14" t="s">
-        <v>104</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="C16" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
adding selective substrates for surrogate models GEMS
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study.xlsx
+++ b/excel files/propionate_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55463684-73A1-4E31-A540-AAADDE38160E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D73252-9236-4342-AC8E-1BA2768D05F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" firstSheet="1" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -798,7 +798,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -856,6 +856,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1138,7 +1145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1235,6 +1242,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3918,8 +3928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE4236-3006-4E07-A9E2-DEE610CD0DBE}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D22" sqref="D21:D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -5592,9 +5602,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6945,9 +6955,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B92B1C5-379D-4587-B23B-6C3AF487A07D}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J35" sqref="J35"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -7669,8 +7679,8 @@
       <c r="J13" s="51">
         <v>0</v>
       </c>
-      <c r="K13" s="53" t="s">
-        <v>25</v>
+      <c r="K13" s="52">
+        <v>0</v>
       </c>
       <c r="L13" s="32">
         <v>0</v>
@@ -7690,8 +7700,8 @@
       <c r="Q13" s="1">
         <v>0</v>
       </c>
-      <c r="R13" s="1">
-        <v>0</v>
+      <c r="R13" s="53" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -8221,7 +8231,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8426,7 +8436,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -8706,7 +8716,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9024,7 +9034,7 @@
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="54" t="s">
         <v>237</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -9053,7 +9063,7 @@
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="54" t="s">
         <v>237</v>
       </c>
       <c r="C14" s="5" t="s">

</xml_diff>